<commit_message>
basic app is done
</commit_message>
<xml_diff>
--- a/Twin Screw Selection Program.xlsx
+++ b/Twin Screw Selection Program.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Desktop/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D25ACB9-3735-C047-A181-04063D7DB7DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51220E24-BAC2-AA48-86A9-E3B0A3DE73A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="21100" windowHeight="15600" xr2:uid="{D7BA4155-18E7-4908-B3BA-4C75047B4766}"/>
   </bookViews>
@@ -20,16 +20,10 @@
     <sheet name="Sheet 5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet 6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -172,10 +166,10 @@
     <t>Optional for Intermediate Value, or take direct from sheet 6</t>
   </si>
   <si>
-    <t>Oeff RPM = (RPM / 1500)^1.6</t>
-  </si>
-  <si>
     <t>Pp=(Sheet 2 * Sheet 6 * Sheet 5)</t>
+  </si>
+  <si>
+    <t>Coeff RPM = (RPM / 1500)^1.6</t>
   </si>
 </sst>
 </file>
@@ -586,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8BA5813-B897-4769-93C0-0C1F12371CAC}">
   <dimension ref="B3:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -669,7 +663,7 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
@@ -686,7 +680,7 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
@@ -738,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55C67C6-4017-4559-BF84-5B2364C41245}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1447,16 +1441,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="D18:D20"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="D43:D44"/>
     <mergeCell ref="A46"/>
@@ -1471,6 +1455,16 @@
     <mergeCell ref="D28:D31"/>
     <mergeCell ref="D32:D35"/>
     <mergeCell ref="D36:D39"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1481,7 +1475,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1581,7 +1575,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1692,9 +1686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA0C8BFA-ACA5-4AE5-8889-EABAA5D5B5D1}">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2333,7 +2325,7 @@
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>